<commit_message>
Updated the valid usn/pswd
</commit_message>
<xml_diff>
--- a/testData/Input/DataExcel.xlsx
+++ b/testData/Input/DataExcel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Invalid_Login" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>MyUserName</t>
   </si>
@@ -77,16 +77,13 @@
     <t>lastPassword112299</t>
   </si>
   <si>
-    <t>myownemailaccount2123@gmail.com</t>
-  </si>
-  <si>
-    <t>india12131415</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>RajGuru11991145@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -465,7 +462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -477,10 +474,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -585,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,18 +594,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>